<commit_message>
api test file update
</commit_message>
<xml_diff>
--- a/StreamLine API Automator/tests/test.xlsx
+++ b/StreamLine API Automator/tests/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\StreamLineQA-Automation-Test\StreamLine API Automator\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4781548-8535-4B4D-A568-7895FC1C5AFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D257C120-7BCF-4C7E-BE44-764439AD343D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -763,7 +763,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,11 +967,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="E2:E10" xr:uid="{BADAA158-2BC8-4252-BE08-38CAEBB42DDA}">
-      <formula1>"equals,contains,has size,has item,is empty,greater than,less than,greater than or equal to,less than or equal to,does not equal,does not contain,does not have item,is not empty,"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="C2:C10" xr:uid="{B56EB8BE-4B25-4655-BD46-921F53583AB3}">
       <formula1>"Response,Body,Status Code"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="E2:E10" xr:uid="{69159E98-96CE-4185-957D-255DB481212A}">
+      <formula1>"equals,equals integer,equals decimal,contains,has size,has item,is empty,greater than,less than,greater than or equal to,less than or equal to,does not equal,does not equal integer,does not equal decimal,does not contain,does not have item,is not empty,"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>